<commit_message>
BaseTypes, Shader, Shader Program
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Initiate project</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Docking</t>
+  </si>
+  <si>
+    <t>Dockspace Menu</t>
+  </si>
+  <si>
+    <t>ShaderProgram</t>
+  </si>
+  <si>
+    <t>ImGui Rendering</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,12 +542,12 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -546,7 +555,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -554,7 +563,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -562,7 +571,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -570,7 +579,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -578,9 +587,33 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Give access to camera target
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Initiate project</t>
   </si>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -643,13 +643,16 @@
       <c r="A14" t="s">
         <v>49</v>
       </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -665,7 +668,7 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,7 +676,7 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -729,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,6 +760,9 @@
       <c r="B28" t="s">
         <v>42</v>
       </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -798,7 +804,7 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,6 +853,9 @@
       <c r="B39" t="s">
         <v>35</v>
       </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -878,11 +887,17 @@
       <c r="B43" t="s">
         <v>39</v>
       </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" t="s">
         <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Give access to Background Color
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>Initiate project</t>
   </si>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,6 +860,9 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
yaml-cpp,  Scene Object  Map
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Initiate project</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Tilemap</t>
+  </si>
+  <si>
+    <t>Cone</t>
+  </si>
+  <si>
+    <t>Cylindre</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,27 +927,39 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="2"/>
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A26:A31"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A45:A48"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">

</xml_diff>

<commit_message>
Entity Registry new member functions
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\C++\Tomato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070858BE-A9A2-49F3-A25C-414B5AA82B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA445ACA-D641-4525-89ED-AD3B968741B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Initiate project</t>
   </si>
@@ -207,13 +207,10 @@
     <t>Draw 3D</t>
   </si>
   <si>
-    <t>Int</t>
-  </si>
-  <si>
-    <t>Float</t>
-  </si>
-  <si>
     <t>MouseToWorldCoords</t>
+  </si>
+  <si>
+    <t>MeshRenderer</t>
   </si>
 </sst>
 </file>
@@ -541,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,33 +1002,15 @@
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" t="s">
+      <c r="A56" t="s">
         <v>60</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" t="s">
-        <v>61</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1041,7 +1020,7 @@
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A53:A55"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Entity Quad Draw with Tilemap
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\C++\Tomato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA445ACA-D641-4525-89ED-AD3B968741B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6EC669-573F-4AF3-9925-3241BAC8B3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="62">
   <si>
     <t>Initiate project</t>
   </si>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,6 +847,9 @@
       <c r="A36" t="s">
         <v>29</v>
       </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -1015,12 +1018,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A53:A55"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A26:A31"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A55"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
DirectXWindow functions: SetSize, SetPos, SetFullscreen
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\C++\Tomato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6EC669-573F-4AF3-9925-3241BAC8B3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0AA842-1A2E-4C42-A97B-BF8AFD837C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>Initiate project</t>
   </si>
@@ -211,6 +211,33 @@
   </si>
   <si>
     <t>MeshRenderer</t>
+  </si>
+  <si>
+    <t>DirectX Implementation</t>
+  </si>
+  <si>
+    <t>OpenGL Implementation</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>VertexBuffer</t>
+  </si>
+  <si>
+    <t>IndexBuffer</t>
+  </si>
+  <si>
+    <t>Shader</t>
+  </si>
+  <si>
+    <t>VertexArray</t>
+  </si>
+  <si>
+    <t>Renderer3D</t>
+  </si>
+  <si>
+    <t>Device</t>
   </si>
 </sst>
 </file>
@@ -538,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +701,9 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1016,8 +1046,152 @@
         <v>60</v>
       </c>
     </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A57:A64"/>
+    <mergeCell ref="A65:A72"/>
     <mergeCell ref="A53:A55"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A26:A31"/>

</xml_diff>